<commit_message>
data cleaning - in medias res
</commit_message>
<xml_diff>
--- a/scenarios-examples/demo/data/factories/cementFactory_withCCS.xlsx
+++ b/scenarios-examples/demo/data/factories/cementFactory_withCCS.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/data/demo/factories/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/wajju/GitHub/BlackBlox/scenarios-examples/demo/data/factories/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{11CD4EB9-7FDE-1942-B0B5-52C9672484CF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0BB957A-98D8-D548-8C3A-A06FC96319EB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="3660" windowWidth="27640" windowHeight="16540" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10760" yWindow="3660" windowWidth="27640" windowHeight="16540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Chain List" sheetId="1" r:id="rId1"/>
@@ -578,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -661,7 +661,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>

</xml_diff>